<commit_message>
Updates from 0409 meeting
Please see README.txt
</commit_message>
<xml_diff>
--- a/outcome/var_relevant_list.xlsx
+++ b/outcome/var_relevant_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsung\Desktop\BIOS\Research_Covid\git\Research_COVID\outcome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311E2A50-EF60-426D-BFD7-642994EE9FEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FEFB87-C3FA-4247-A53A-A3F9DE931204}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B310FCD2-898F-41EC-8397-259732FF0A30}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>variable_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,10 +85,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>in R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cowin_vaccine_data_statewise</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -116,6 +112,83 @@
   <si>
     <t>no missing</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hostpital_public</t>
+  </si>
+  <si>
+    <t>hospital_private</t>
+  </si>
+  <si>
+    <t>hospital_total</t>
+  </si>
+  <si>
+    <t>hospital_beds_public</t>
+  </si>
+  <si>
+    <t>hospital_beds_private</t>
+  </si>
+  <si>
+    <t>hospital_beds_total</t>
+  </si>
+  <si>
+    <t>icu_beds_public</t>
+  </si>
+  <si>
+    <t>icu_beds_private</t>
+  </si>
+  <si>
+    <t>icu_beds_total</t>
+  </si>
+  <si>
+    <t>ventilators_public</t>
+  </si>
+  <si>
+    <t>ventilators_private</t>
+  </si>
+  <si>
+    <t>ventilators_total</t>
+  </si>
+  <si>
+    <t>hostpital_capacity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2020.pdf'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2021.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2022.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2023.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2024.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2025.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2026.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2027.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2028.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2029.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2030.pdf'</t>
+  </si>
+  <si>
+    <t>from 'State-wise-estimates-of-current-beds-and-ventilators_24Apr2031.pdf'</t>
   </si>
 </sst>
 </file>
@@ -479,19 +552,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FE40C9-FFE7-4DA8-A5F2-016A4BCFBD73}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,13 +579,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -519,10 +591,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -536,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -550,7 +622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -564,7 +636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -578,7 +650,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -592,7 +664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -606,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -620,12 +692,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -634,12 +706,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -648,18 +720,186 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -684,12 +924,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>